<commit_message>
This stable version where are all functions and experiments: adding mp3 files into DB; can add images into DB and can check if are the same by their HASH; can send to you random image from DB; can work with pandas - helps with reporting by excel files. It hosted on pythonanywhere.com
</commit_message>
<xml_diff>
--- a/files/spents.xlsx
+++ b/files/spents.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="33">
   <si>
     <t>Дата</t>
   </si>
@@ -51,13 +51,25 @@
     <t>Одежда</t>
   </si>
   <si>
+    <t>Связь</t>
+  </si>
+  <si>
+    <t>Велики</t>
+  </si>
+  <si>
+    <t>Алкоголь</t>
+  </si>
+  <si>
+    <t>Здоровье</t>
+  </si>
+  <si>
     <t>Прочее</t>
   </si>
   <si>
-    <t>Связь</t>
+    <t>Комменты</t>
   </si>
   <si>
-    <t>Комменты</t>
+    <t>Зоровье</t>
   </si>
   <si>
     <t>пистолеты</t>
@@ -82,6 +94,36 @@
   </si>
   <si>
     <t>happy bike lane</t>
+  </si>
+  <si>
+    <t>велики</t>
+  </si>
+  <si>
+    <t>чистка зубов</t>
+  </si>
+  <si>
+    <t>сигареты; ракетки + очки + сковорода и иже с ними</t>
+  </si>
+  <si>
+    <t>сигареты</t>
+  </si>
+  <si>
+    <t>vpn redshield; подарки для детей</t>
+  </si>
+  <si>
+    <t>лечу голову  в патайске</t>
+  </si>
+  <si>
+    <t>панииииирррр ооааооо ммм))0)</t>
+  </si>
+  <si>
+    <t>свет + вода; билеты</t>
+  </si>
+  <si>
+    <t>велики, дорога к ним, вся еда, бургер Кинг,  весь севен (нет алкоголя)</t>
+  </si>
+  <si>
+    <t>инет</t>
   </si>
 </sst>
 </file>
@@ -443,13 +485,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K32"/>
+  <dimension ref="A1:N32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -483,78 +525,87 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:11">
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" s="2">
         <v>44927</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:14">
       <c r="A3" s="2">
         <v>44928</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:14">
       <c r="A4" s="2">
         <v>44929</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:14">
       <c r="A5" s="2">
         <v>44930</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:14">
       <c r="A6" s="2">
         <v>44931</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:14">
       <c r="A7" s="2">
         <v>44932</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:14">
       <c r="A8" s="2">
         <v>44933</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:14">
       <c r="A9" s="2">
         <v>44934</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:14">
       <c r="A10" s="2">
         <v>44935</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:14">
       <c r="A11" s="2">
         <v>44936</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:14">
       <c r="A12" s="2">
         <v>44937</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:14">
       <c r="A13" s="2">
         <v>44938</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:14">
       <c r="A14" s="2">
         <v>44939</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:14">
       <c r="A15" s="2">
         <v>44940</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:14">
       <c r="A16" s="2">
         <v>44941</v>
       </c>
@@ -646,13 +697,13 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K32"/>
+  <dimension ref="A1:N32"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -686,78 +737,87 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:11">
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" s="2">
         <v>45200</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:14">
       <c r="A3" s="2">
         <v>45201</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:14">
       <c r="A4" s="2">
         <v>45202</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:14">
       <c r="A5" s="2">
         <v>45203</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:14">
       <c r="A6" s="2">
         <v>45204</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:14">
       <c r="A7" s="2">
         <v>45205</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:14">
       <c r="A8" s="2">
         <v>45206</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:14">
       <c r="A9" s="2">
         <v>45207</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:14">
       <c r="A10" s="2">
         <v>45208</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:14">
       <c r="A11" s="2">
         <v>45209</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:14">
       <c r="A12" s="2">
         <v>45210</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:14">
       <c r="A13" s="2">
         <v>45211</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:14">
       <c r="A14" s="2">
         <v>45212</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:14">
       <c r="A15" s="2">
         <v>45213</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:14">
       <c r="A16" s="2">
         <v>45214</v>
       </c>
@@ -849,13 +909,13 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K31"/>
+  <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -889,78 +949,87 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:11">
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" s="2">
         <v>45231</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:14">
       <c r="A3" s="2">
         <v>45232</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:14">
       <c r="A4" s="2">
         <v>45233</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:14">
       <c r="A5" s="2">
         <v>45234</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:14">
       <c r="A6" s="2">
         <v>45235</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:14">
       <c r="A7" s="2">
         <v>45236</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:14">
       <c r="A8" s="2">
         <v>45237</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:14">
       <c r="A9" s="2">
         <v>45238</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:14">
       <c r="A10" s="2">
         <v>45239</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:14">
       <c r="A11" s="2">
         <v>45240</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:14">
       <c r="A12" s="2">
         <v>45241</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:14">
       <c r="A13" s="2">
         <v>45242</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:14">
       <c r="A14" s="2">
         <v>45243</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:14">
       <c r="A15" s="2">
         <v>45244</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:14">
       <c r="A16" s="2">
         <v>45245</v>
       </c>
@@ -1047,13 +1116,13 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K32"/>
+  <dimension ref="A1:N32"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1087,78 +1156,87 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:11">
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" s="2">
         <v>45261</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:14">
       <c r="A3" s="2">
         <v>45262</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:14">
       <c r="A4" s="2">
         <v>45263</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:14">
       <c r="A5" s="2">
         <v>45264</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:14">
       <c r="A6" s="2">
         <v>45265</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:14">
       <c r="A7" s="2">
         <v>45266</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:14">
       <c r="A8" s="2">
         <v>45267</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:14">
       <c r="A9" s="2">
         <v>45268</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:14">
       <c r="A10" s="2">
         <v>45269</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:14">
       <c r="A11" s="2">
         <v>45270</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:14">
       <c r="A12" s="2">
         <v>45271</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:14">
       <c r="A13" s="2">
         <v>45272</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:14">
       <c r="A14" s="2">
         <v>45273</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:14">
       <c r="A15" s="2">
         <v>45274</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:14">
       <c r="A16" s="2">
         <v>45275</v>
       </c>
@@ -1250,13 +1328,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K32"/>
+  <dimension ref="A1:N29"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1290,160 +1368,154 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:11">
+      <c r="L1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" s="2">
-        <v>44927</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
+        <v>44958</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" s="2">
-        <v>44928</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
+        <v>44959</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4" s="2">
-        <v>44929</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
+        <v>44960</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
       <c r="A5" s="2">
-        <v>44930</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
+        <v>44961</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
       <c r="A6" s="2">
-        <v>44931</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
+        <v>44962</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
       <c r="A7" s="2">
-        <v>44932</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
+        <v>44963</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
       <c r="A8" s="2">
-        <v>44933</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
+        <v>44964</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
       <c r="A9" s="2">
-        <v>44934</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11">
+        <v>44965</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
       <c r="A10" s="2">
-        <v>44935</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
+        <v>44966</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
       <c r="A11" s="2">
-        <v>44936</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11">
+        <v>44967</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
       <c r="A12" s="2">
-        <v>44937</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
+        <v>44968</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
       <c r="A13" s="2">
-        <v>44938</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11">
+        <v>44969</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
       <c r="A14" s="2">
-        <v>44939</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11">
+        <v>44970</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
       <c r="A15" s="2">
-        <v>44940</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11">
+        <v>44971</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
       <c r="A16" s="2">
-        <v>44941</v>
+        <v>44972</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" s="2">
-        <v>44942</v>
+        <v>44973</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" s="2">
-        <v>44943</v>
+        <v>44974</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" s="2">
-        <v>44944</v>
+        <v>44975</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" s="2">
-        <v>44945</v>
+        <v>44976</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" s="2">
-        <v>44946</v>
+        <v>44977</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" s="2">
-        <v>44947</v>
+        <v>44978</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" s="2">
-        <v>44948</v>
+        <v>44979</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" s="2">
-        <v>44949</v>
+        <v>44980</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" s="2">
-        <v>44950</v>
+        <v>44981</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" s="2">
-        <v>44951</v>
+        <v>44982</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" s="2">
-        <v>44952</v>
+        <v>44983</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" s="2">
-        <v>44953</v>
+        <v>44984</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" s="2">
-        <v>44954</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1">
-      <c r="A30" s="2">
-        <v>44955</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1">
-      <c r="A31" s="2">
-        <v>44956</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1">
-      <c r="A32" s="2">
-        <v>44957</v>
+        <v>44985</v>
       </c>
     </row>
   </sheetData>
@@ -1453,13 +1525,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K32"/>
+  <dimension ref="A1:N32"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1493,160 +1565,169 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:11">
+      <c r="L1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" s="2">
-        <v>44927</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
+        <v>44986</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" s="2">
-        <v>44928</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
+        <v>44987</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4" s="2">
-        <v>44929</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
+        <v>44988</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
       <c r="A5" s="2">
-        <v>44930</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
+        <v>44989</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
       <c r="A6" s="2">
-        <v>44931</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
+        <v>44990</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
       <c r="A7" s="2">
-        <v>44932</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
+        <v>44991</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
       <c r="A8" s="2">
-        <v>44933</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
+        <v>44992</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
       <c r="A9" s="2">
-        <v>44934</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11">
+        <v>44993</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
       <c r="A10" s="2">
-        <v>44935</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
+        <v>44994</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
       <c r="A11" s="2">
-        <v>44936</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11">
+        <v>44995</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
       <c r="A12" s="2">
-        <v>44937</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
+        <v>44996</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
       <c r="A13" s="2">
-        <v>44938</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11">
+        <v>44997</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
       <c r="A14" s="2">
-        <v>44939</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11">
+        <v>44998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
       <c r="A15" s="2">
-        <v>44940</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11">
+        <v>44999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
       <c r="A16" s="2">
-        <v>44941</v>
+        <v>45000</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" s="2">
-        <v>44942</v>
+        <v>45001</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" s="2">
-        <v>44943</v>
+        <v>45002</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" s="2">
-        <v>44944</v>
+        <v>45003</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" s="2">
-        <v>44945</v>
+        <v>45004</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" s="2">
-        <v>44946</v>
+        <v>45005</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" s="2">
-        <v>44947</v>
+        <v>45006</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" s="2">
-        <v>44948</v>
+        <v>45007</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" s="2">
-        <v>44949</v>
+        <v>45008</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" s="2">
-        <v>44950</v>
+        <v>45009</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" s="2">
-        <v>44951</v>
+        <v>45010</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" s="2">
-        <v>44952</v>
+        <v>45011</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" s="2">
-        <v>44953</v>
+        <v>45012</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" s="2">
-        <v>44954</v>
+        <v>45013</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" s="2">
-        <v>44955</v>
+        <v>45014</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" s="2">
-        <v>44956</v>
+        <v>45015</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" s="2">
-        <v>44957</v>
+        <v>45016</v>
       </c>
     </row>
   </sheetData>
@@ -1656,13 +1737,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K25"/>
+  <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1696,38 +1777,47 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:11">
+      <c r="L1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" s="2">
         <v>45023</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:14">
       <c r="A3" s="2">
         <v>45024</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:14">
       <c r="A4" s="2">
         <v>45025</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:14">
       <c r="A5" s="2">
         <v>45026</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:14">
       <c r="A6" s="2">
         <v>45027</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:14">
       <c r="A7" s="2">
         <v>45028</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:14">
       <c r="A8" s="2">
         <v>45029</v>
       </c>
@@ -1738,7 +1828,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:14">
       <c r="A9" s="2">
         <v>45030</v>
       </c>
@@ -1752,10 +1842,10 @@
         <v>390</v>
       </c>
       <c r="K9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
       <c r="A10" s="2">
         <v>45031</v>
       </c>
@@ -1766,7 +1856,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:14">
       <c r="A11" s="2">
         <v>45032</v>
       </c>
@@ -1786,10 +1876,10 @@
         <v>100</v>
       </c>
       <c r="K11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
       <c r="A12" s="2">
         <v>45033</v>
       </c>
@@ -1809,25 +1899,25 @@
         <v>600</v>
       </c>
       <c r="K12" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
       <c r="A13" s="2">
         <v>45034</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:14">
       <c r="A14" s="2">
         <v>45035</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:14">
       <c r="A15" s="2">
         <v>45036</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:14">
       <c r="A16" s="2">
         <v>45037</v>
       </c>
@@ -1884,13 +1974,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K32"/>
+  <dimension ref="A1:N32"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1924,23 +2014,32 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:11">
+      <c r="L1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" s="2">
         <v>45047</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:14">
       <c r="A3" s="2">
         <v>45048</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:14">
       <c r="A4" s="2">
         <v>45049</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:14">
       <c r="A5" s="2">
         <v>45050</v>
       </c>
@@ -1953,28 +2052,28 @@
       <c r="H5">
         <v>220</v>
       </c>
-      <c r="I5">
+      <c r="M5">
         <v>350</v>
       </c>
-      <c r="K5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
+      <c r="N5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
       <c r="A6" s="2">
         <v>45051</v>
       </c>
       <c r="B6">
         <v>398</v>
       </c>
-      <c r="I6">
+      <c r="M6">
         <v>100</v>
       </c>
-      <c r="K6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
+      <c r="N6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
       <c r="A7" s="2">
         <v>45052</v>
       </c>
@@ -1987,14 +2086,14 @@
       <c r="H7">
         <v>3150</v>
       </c>
-      <c r="I7">
+      <c r="M7">
         <v>1420</v>
       </c>
-      <c r="K7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
+      <c r="N7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
       <c r="A8" s="2">
         <v>45053</v>
       </c>
@@ -2010,11 +2109,11 @@
       <c r="G8">
         <v>1250</v>
       </c>
-      <c r="J8">
+      <c r="I8">
         <v>310</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:14">
       <c r="A9" s="2">
         <v>45054</v>
       </c>
@@ -2031,12 +2130,12 @@
         <v>550</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:14">
       <c r="A10" s="2">
         <v>45055</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:14">
       <c r="A11" s="2">
         <v>45056</v>
       </c>
@@ -2047,12 +2146,12 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:14">
       <c r="A12" s="2">
         <v>45057</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:14">
       <c r="A13" s="2">
         <v>45058</v>
       </c>
@@ -2062,14 +2161,14 @@
       <c r="G13">
         <v>1400</v>
       </c>
-      <c r="I13">
+      <c r="M13">
         <v>550</v>
       </c>
-      <c r="K13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11">
+      <c r="N13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
       <c r="A14" s="2">
         <v>45059</v>
       </c>
@@ -2077,7 +2176,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:14">
       <c r="A15" s="2">
         <v>45060</v>
       </c>
@@ -2093,97 +2192,151 @@
       <c r="G15">
         <v>1000</v>
       </c>
-      <c r="I15">
+      <c r="M15">
         <v>840</v>
       </c>
-      <c r="K15" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11">
+      <c r="N15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
       <c r="A16" s="2">
         <v>45061</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:14">
       <c r="A17" s="2">
         <v>45062</v>
       </c>
       <c r="B17">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
+        <v>540</v>
+      </c>
+      <c r="E17">
+        <v>350</v>
+      </c>
+      <c r="G17">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
       <c r="A18" s="2">
         <v>45063</v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
+      <c r="B18">
+        <v>275</v>
+      </c>
+      <c r="C18">
+        <v>580</v>
+      </c>
+      <c r="F18">
+        <v>400</v>
+      </c>
+      <c r="G18">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
       <c r="A19" s="2">
         <v>45064</v>
       </c>
-    </row>
-    <row r="20" spans="1:2">
+      <c r="B19">
+        <v>200</v>
+      </c>
+      <c r="E19">
+        <v>211</v>
+      </c>
+      <c r="G19">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
       <c r="A20" s="2">
         <v>45065</v>
       </c>
-    </row>
-    <row r="21" spans="1:2">
+      <c r="B20">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
       <c r="A21" s="2">
         <v>45066</v>
       </c>
-    </row>
-    <row r="22" spans="1:2">
+      <c r="B21">
+        <v>350</v>
+      </c>
+      <c r="F21">
+        <v>800</v>
+      </c>
+      <c r="M21">
+        <v>840</v>
+      </c>
+      <c r="N21" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
       <c r="A22" s="2">
         <v>45067</v>
       </c>
-    </row>
-    <row r="23" spans="1:2">
+      <c r="E22">
+        <v>100</v>
+      </c>
+      <c r="F22">
+        <v>217</v>
+      </c>
+      <c r="M22">
+        <v>2000</v>
+      </c>
+      <c r="N22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
       <c r="A23" s="2">
         <v>45068</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:14">
       <c r="A24" s="2">
         <v>45069</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:14">
       <c r="A25" s="2">
         <v>45070</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:14">
       <c r="A26" s="2">
         <v>45071</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:14">
       <c r="A27" s="2">
         <v>45072</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:14">
       <c r="A28" s="2">
         <v>45073</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:14">
       <c r="A29" s="2">
         <v>45074</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:14">
       <c r="A30" s="2">
         <v>45075</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:14">
       <c r="A31" s="2">
         <v>45076</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:14">
       <c r="A32" s="2">
         <v>45077</v>
       </c>
@@ -2195,13 +2348,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K31"/>
+  <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2235,155 +2388,233 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:11">
+      <c r="L1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" s="2">
         <v>45078</v>
       </c>
-    </row>
-    <row r="3" spans="1:11">
+      <c r="B2">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" s="2">
         <v>45079</v>
       </c>
-    </row>
-    <row r="4" spans="1:11">
+      <c r="B3">
+        <v>129</v>
+      </c>
+      <c r="C3">
+        <v>1000</v>
+      </c>
+      <c r="F3">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4" s="2">
         <v>45080</v>
       </c>
-    </row>
-    <row r="5" spans="1:11">
+      <c r="B4">
+        <v>421</v>
+      </c>
+      <c r="F4">
+        <v>120</v>
+      </c>
+      <c r="H4">
+        <v>900</v>
+      </c>
+      <c r="M4">
+        <v>2000</v>
+      </c>
+      <c r="N4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
       <c r="A5" s="2">
         <v>45081</v>
       </c>
-    </row>
-    <row r="6" spans="1:11">
+      <c r="B5">
+        <v>1510</v>
+      </c>
+      <c r="D5">
+        <v>80</v>
+      </c>
+      <c r="F5">
+        <v>350</v>
+      </c>
+      <c r="M5">
+        <v>150</v>
+      </c>
+      <c r="N5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
       <c r="A6" s="2">
         <v>45082</v>
       </c>
-    </row>
-    <row r="7" spans="1:11">
+      <c r="B6">
+        <v>95</v>
+      </c>
+      <c r="F6">
+        <v>190</v>
+      </c>
+      <c r="M6">
+        <v>2800</v>
+      </c>
+      <c r="N6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
       <c r="A7" s="2">
         <v>45083</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:14">
       <c r="A8" s="2">
         <v>45084</v>
       </c>
-    </row>
-    <row r="9" spans="1:11">
+      <c r="B8">
+        <v>130</v>
+      </c>
+      <c r="D8">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
       <c r="A9" s="2">
         <v>45085</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:14">
       <c r="A10" s="2">
         <v>45086</v>
       </c>
-    </row>
-    <row r="11" spans="1:11">
+      <c r="B10">
+        <v>230</v>
+      </c>
+      <c r="D10">
+        <v>2860</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
       <c r="A11" s="2">
         <v>45087</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:14">
       <c r="A12" s="2">
         <v>45088</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:14">
       <c r="A13" s="2">
         <v>45089</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:14">
       <c r="A14" s="2">
         <v>45090</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:14">
       <c r="A15" s="2">
         <v>45091</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:14">
       <c r="A16" s="2">
         <v>45092</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:2">
       <c r="A17" s="2">
         <v>45093</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:2">
       <c r="A18" s="2">
         <v>45094</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:2">
       <c r="A19" s="2">
         <v>45095</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:2">
       <c r="A20" s="2">
         <v>45096</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
+    <row r="21" spans="1:2">
       <c r="A21" s="2">
         <v>45097</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
+    <row r="22" spans="1:2">
       <c r="A22" s="2">
         <v>45098</v>
       </c>
     </row>
-    <row r="23" spans="1:1">
+    <row r="23" spans="1:2">
       <c r="A23" s="2">
         <v>45099</v>
       </c>
     </row>
-    <row r="24" spans="1:1">
+    <row r="24" spans="1:2">
       <c r="A24" s="2">
         <v>45100</v>
       </c>
     </row>
-    <row r="25" spans="1:1">
+    <row r="25" spans="1:2">
       <c r="A25" s="2">
         <v>45101</v>
       </c>
     </row>
-    <row r="26" spans="1:1">
+    <row r="26" spans="1:2">
       <c r="A26" s="2">
         <v>45102</v>
       </c>
     </row>
-    <row r="27" spans="1:1">
+    <row r="27" spans="1:2">
       <c r="A27" s="2">
         <v>45103</v>
       </c>
     </row>
-    <row r="28" spans="1:1">
+    <row r="28" spans="1:2">
       <c r="A28" s="2">
         <v>45104</v>
       </c>
     </row>
-    <row r="29" spans="1:1">
+    <row r="29" spans="1:2">
       <c r="A29" s="2">
         <v>45105</v>
       </c>
     </row>
-    <row r="30" spans="1:1">
+    <row r="30" spans="1:2">
       <c r="A30" s="2">
         <v>45106</v>
       </c>
     </row>
-    <row r="31" spans="1:1">
+    <row r="31" spans="1:2">
       <c r="A31" s="2">
         <v>45107</v>
+      </c>
+      <c r="B31">
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -2393,13 +2624,13 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K32"/>
+  <dimension ref="A1:N32"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2433,158 +2664,368 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:11">
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" s="2">
         <v>45108</v>
       </c>
-    </row>
-    <row r="3" spans="1:11">
+      <c r="B2">
+        <v>400</v>
+      </c>
+      <c r="D2">
+        <v>900</v>
+      </c>
+      <c r="F2">
+        <v>358</v>
+      </c>
+      <c r="G2">
+        <v>770</v>
+      </c>
+      <c r="I2">
+        <v>360</v>
+      </c>
+      <c r="J2">
+        <v>160</v>
+      </c>
+      <c r="K2">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" s="2">
         <v>45109</v>
       </c>
-    </row>
-    <row r="4" spans="1:11">
+      <c r="B3">
+        <v>135</v>
+      </c>
+      <c r="D3">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4" s="2">
         <v>45110</v>
       </c>
-    </row>
-    <row r="5" spans="1:11">
+      <c r="B4">
+        <v>350</v>
+      </c>
+      <c r="E4">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
       <c r="A5" s="2">
         <v>45111</v>
       </c>
-    </row>
-    <row r="6" spans="1:11">
+      <c r="B5">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
       <c r="A6" s="2">
         <v>45112</v>
       </c>
-    </row>
-    <row r="7" spans="1:11">
+      <c r="B6">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
       <c r="A7" s="2">
         <v>45113</v>
       </c>
-    </row>
-    <row r="8" spans="1:11">
+      <c r="B7">
+        <v>267</v>
+      </c>
+      <c r="E7">
+        <v>182</v>
+      </c>
+      <c r="K7">
+        <v>78</v>
+      </c>
+      <c r="M7">
+        <v>1550</v>
+      </c>
+      <c r="N7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
       <c r="A8" s="2">
         <v>45114</v>
       </c>
-    </row>
-    <row r="9" spans="1:11">
+      <c r="B8">
+        <v>225</v>
+      </c>
+      <c r="E8">
+        <v>50</v>
+      </c>
+      <c r="F8">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
       <c r="A9" s="2">
         <v>45115</v>
       </c>
-    </row>
-    <row r="10" spans="1:11">
+      <c r="B9">
+        <v>80</v>
+      </c>
+      <c r="D9">
+        <v>268</v>
+      </c>
+      <c r="E9">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
       <c r="A10" s="2">
         <v>45116</v>
       </c>
-    </row>
-    <row r="11" spans="1:11">
+      <c r="B10">
+        <v>120</v>
+      </c>
+      <c r="D10">
+        <v>713</v>
+      </c>
+      <c r="E10">
+        <v>216</v>
+      </c>
+      <c r="F10">
+        <v>624</v>
+      </c>
+      <c r="I10">
+        <v>330</v>
+      </c>
+      <c r="J10">
+        <v>420</v>
+      </c>
+      <c r="L10">
+        <v>1059</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
       <c r="A11" s="2">
         <v>45117</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:14">
       <c r="A12" s="2">
         <v>45118</v>
       </c>
-    </row>
-    <row r="13" spans="1:11">
+      <c r="B12">
+        <v>1020</v>
+      </c>
+      <c r="D12">
+        <v>212</v>
+      </c>
+      <c r="E12">
+        <v>670</v>
+      </c>
+      <c r="G12">
+        <v>640</v>
+      </c>
+      <c r="K12">
+        <v>430</v>
+      </c>
+      <c r="M12">
+        <v>430</v>
+      </c>
+      <c r="N12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
       <c r="A13" s="2">
         <v>45119</v>
       </c>
-    </row>
-    <row r="14" spans="1:11">
+      <c r="F13">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
       <c r="A14" s="2">
         <v>45120</v>
       </c>
-    </row>
-    <row r="15" spans="1:11">
+      <c r="B14">
+        <v>565</v>
+      </c>
+      <c r="E14">
+        <v>176</v>
+      </c>
+      <c r="F14">
+        <v>165</v>
+      </c>
+      <c r="K14">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
       <c r="A15" s="2">
         <v>45121</v>
       </c>
-    </row>
-    <row r="16" spans="1:11">
+      <c r="B15">
+        <v>789</v>
+      </c>
+      <c r="K15">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
       <c r="A16" s="2">
         <v>45122</v>
       </c>
-    </row>
-    <row r="17" spans="1:1">
+      <c r="B16">
+        <v>690</v>
+      </c>
+      <c r="E16">
+        <v>30</v>
+      </c>
+      <c r="F16">
+        <v>260</v>
+      </c>
+      <c r="K16">
+        <v>120</v>
+      </c>
+      <c r="M16">
+        <v>2650</v>
+      </c>
+      <c r="N16" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
       <c r="A17" s="2">
         <v>45123</v>
       </c>
-    </row>
-    <row r="18" spans="1:1">
+      <c r="B17">
+        <v>130</v>
+      </c>
+      <c r="D17">
+        <v>100</v>
+      </c>
+      <c r="F17">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
       <c r="A18" s="2">
         <v>45124</v>
       </c>
-    </row>
-    <row r="19" spans="1:1">
+      <c r="B18">
+        <v>771</v>
+      </c>
+      <c r="E18">
+        <v>30</v>
+      </c>
+      <c r="M18">
+        <v>1700</v>
+      </c>
+      <c r="N18" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
       <c r="A19" s="2">
         <v>45125</v>
       </c>
-    </row>
-    <row r="20" spans="1:1">
+      <c r="B19">
+        <v>605</v>
+      </c>
+      <c r="E19">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
       <c r="A20" s="2">
         <v>45126</v>
       </c>
-    </row>
-    <row r="21" spans="1:1">
+      <c r="B20">
+        <v>720</v>
+      </c>
+      <c r="D20">
+        <v>1130</v>
+      </c>
+      <c r="F20">
+        <v>70</v>
+      </c>
+      <c r="M20">
+        <v>850</v>
+      </c>
+      <c r="N20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
       <c r="A21" s="2">
         <v>45127</v>
       </c>
-    </row>
-    <row r="22" spans="1:1">
+      <c r="G21">
+        <v>600</v>
+      </c>
+      <c r="K21">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
       <c r="A22" s="2">
         <v>45128</v>
       </c>
     </row>
-    <row r="23" spans="1:1">
+    <row r="23" spans="1:14">
       <c r="A23" s="2">
         <v>45129</v>
       </c>
     </row>
-    <row r="24" spans="1:1">
+    <row r="24" spans="1:14">
       <c r="A24" s="2">
         <v>45130</v>
       </c>
     </row>
-    <row r="25" spans="1:1">
+    <row r="25" spans="1:14">
       <c r="A25" s="2">
         <v>45131</v>
       </c>
     </row>
-    <row r="26" spans="1:1">
+    <row r="26" spans="1:14">
       <c r="A26" s="2">
         <v>45132</v>
       </c>
     </row>
-    <row r="27" spans="1:1">
+    <row r="27" spans="1:14">
       <c r="A27" s="2">
         <v>45133</v>
       </c>
     </row>
-    <row r="28" spans="1:1">
+    <row r="28" spans="1:14">
       <c r="A28" s="2">
         <v>45134</v>
       </c>
     </row>
-    <row r="29" spans="1:1">
+    <row r="29" spans="1:14">
       <c r="A29" s="2">
         <v>45135</v>
       </c>
     </row>
-    <row r="30" spans="1:1">
+    <row r="30" spans="1:14">
       <c r="A30" s="2">
         <v>45136</v>
       </c>
     </row>
-    <row r="31" spans="1:1">
+    <row r="31" spans="1:14">
       <c r="A31" s="2">
         <v>45137</v>
       </c>
     </row>
-    <row r="32" spans="1:1">
+    <row r="32" spans="1:14">
       <c r="A32" s="2">
         <v>45138</v>
       </c>
@@ -2596,13 +3037,13 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K32"/>
+  <dimension ref="A1:N32"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2636,78 +3077,87 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:11">
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" s="2">
         <v>45139</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:14">
       <c r="A3" s="2">
         <v>45140</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:14">
       <c r="A4" s="2">
         <v>45141</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:14">
       <c r="A5" s="2">
         <v>45142</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:14">
       <c r="A6" s="2">
         <v>45143</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:14">
       <c r="A7" s="2">
         <v>45144</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:14">
       <c r="A8" s="2">
         <v>45145</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:14">
       <c r="A9" s="2">
         <v>45146</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:14">
       <c r="A10" s="2">
         <v>45147</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:14">
       <c r="A11" s="2">
         <v>45148</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:14">
       <c r="A12" s="2">
         <v>45149</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:14">
       <c r="A13" s="2">
         <v>45150</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:14">
       <c r="A14" s="2">
         <v>45151</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:14">
       <c r="A15" s="2">
         <v>45152</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:14">
       <c r="A16" s="2">
         <v>45153</v>
       </c>
@@ -2799,13 +3249,13 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K31"/>
+  <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2839,78 +3289,87 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:11">
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" s="2">
         <v>45170</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:14">
       <c r="A3" s="2">
         <v>45171</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:14">
       <c r="A4" s="2">
         <v>45172</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:14">
       <c r="A5" s="2">
         <v>45173</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:14">
       <c r="A6" s="2">
         <v>45174</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:14">
       <c r="A7" s="2">
         <v>45175</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:14">
       <c r="A8" s="2">
         <v>45176</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:14">
       <c r="A9" s="2">
         <v>45177</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:14">
       <c r="A10" s="2">
         <v>45178</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:14">
       <c r="A11" s="2">
         <v>45179</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:14">
       <c r="A12" s="2">
         <v>45180</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:14">
       <c r="A13" s="2">
         <v>45181</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:14">
       <c r="A14" s="2">
         <v>45182</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:14">
       <c r="A15" s="2">
         <v>45183</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:14">
       <c r="A16" s="2">
         <v>45184</v>
       </c>

</xml_diff>